<commit_message>
Modificacion prueba a original
Restaurar datos originales Plan Cuentas
</commit_message>
<xml_diff>
--- a/EDS001.xlsx
+++ b/EDS001.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\TRABAJO\wefinz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MANUELW10-OFICINA\Documents\GitHub\wefinz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8D18E1-2AEF-4B7C-B932-75AE1B3D34EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEED450-1EC4-4D42-95DB-EAF48E9B1DA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7C39CDB8-AC8A-40A6-A4EA-995BF854F855}"/>
   </bookViews>
@@ -2532,7 +2532,7 @@
     <t>TRANSFERENCIA POR DETERIORO DE AJUSTES VALORATIVOS NEGATIVOS PREVIOS, EMPRESAS ASOCIADAS</t>
   </si>
   <si>
-    <t>CARGA DE DATOSz</t>
+    <t>CARGA DE DATOS</t>
   </si>
 </sst>
 </file>
@@ -2935,7 +2935,7 @@
   <dimension ref="A1:C838"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A811" workbookViewId="0">
-      <selection activeCell="C839" sqref="C839"/>
+      <selection activeCell="C838" sqref="C838"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>